<commit_message>
sync with main repo
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/Create Engineering Item Master.xlsx
+++ b/templates/AutomationOrg/Create Engineering Item Master.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="144">
   <si>
     <t>Item Number</t>
   </si>
@@ -454,6 +454,24 @@
   </si>
   <si>
     <t>a345f000000uafrAAA</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-M72O3</t>
+  </si>
+  <si>
+    <t>a345f000000uau8AAA</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-N4EN6</t>
+  </si>
+  <si>
+    <t>a345f000000uauDAAQ</t>
+  </si>
+  <si>
+    <t>Pro-PEItem-NXQGE</t>
+  </si>
+  <si>
+    <t>a345f000000uauIAAQ</t>
   </si>
 </sst>
 </file>
@@ -464,7 +482,7 @@
     <numFmt numFmtId="164" formatCode="mm\/dd\/yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +510,42 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -634,7 +688,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -675,11 +729,20 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -705,8 +768,14 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="9" fillId="0" fontId="21" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="22" numFmtId="165" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="10" fillId="0" fontId="23" numFmtId="49" xfId="0"/>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="11" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="24" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="11" fillId="0" fontId="25" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="26" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="12" fillId="0" fontId="27" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="28" numFmtId="165" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="13" fillId="0" fontId="29" numFmtId="49" xfId="0"/>
+    <xf numFmtId="165" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="14" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -1141,9 +1210,9 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.01953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.3046875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.26171875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.7421875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1165,13 +1234,13 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
         <v>112</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>